<commit_message>
[BI-1068] Tags header for testing case-sensitivity
</commit_message>
<xml_diff>
--- a/src/files/TraitImport_v03/test_traits_case_insensitivity.xlsx
+++ b/src/files/TraitImport_v03/test_traits_case_insensitivity.xlsx
@@ -113,7 +113,7 @@
     <t>comPUTation</t>
   </si>
   <si>
-    <t>Tags</t>
+    <t>TaGs</t>
   </si>
 </sst>
 </file>
@@ -599,6 +599,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006D74C1D9EC8A1042A5EF45985DF3E9E4" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2000d971e1751a7db8d92151125d08a9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="aa5be1c8-7296-4b7a-853c-c6802fcefdea" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a4a1f299a0d30015388c519f6ad441cc" ns3:_="">
     <xsd:import namespace="aa5be1c8-7296-4b7a-853c-c6802fcefdea"/>
@@ -776,15 +785,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -792,6 +792,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7613A94-47D1-485D-A76D-D3A6CFAB63B4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{340A8394-9E0A-435F-BF61-25A36768AA02}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -809,14 +817,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7613A94-47D1-485D-A76D-D3A6CFAB63B4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EFE1791-BEC8-419B-A7D8-F7EAC9E3F094}">
   <ds:schemaRefs>

</xml_diff>